<commit_message>
Removed Charm of the Mage and Charm of the Seeker Added Charm of Energy, Charm of Fortune and Charm of Stamina instead
</commit_message>
<xml_diff>
--- a/Global/Excel/ItemStatCost.xlsx
+++ b/Global/Excel/ItemStatCost.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Games\Diablo II LOD\data\Global\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF453183-ECDF-42E0-A610-B05D1A58C19B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE89EFA-D4C0-4A01-AF5A-CBCC15D4E422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ItemStatCost" sheetId="1" r:id="rId1"/>
+    <sheet name="ValueRange" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="556">
   <si>
     <t>Stat</t>
   </si>
@@ -1682,12 +1695,20 @@
   </si>
   <si>
     <t>passive_mag_pierce</t>
+  </si>
+  <si>
+    <t>Min</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Max</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2632,7 +2653,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BA360"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -19282,4 +19303,4702 @@
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E135CB1C-A62B-40C9-A4A8-2CBDE7FAF2B1}">
+  <dimension ref="A1:C360"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>554</v>
+      </c>
+      <c r="C1" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2">
+        <f>-ItemStatCost!W2</f>
+        <v>-32</v>
+      </c>
+      <c r="C2">
+        <f>POWER(2,ItemStatCost!V2)-ItemStatCost!W2</f>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3">
+        <f>-ItemStatCost!W3</f>
+        <v>-32</v>
+      </c>
+      <c r="C3">
+        <f>POWER(2,ItemStatCost!V3)-ItemStatCost!W3</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4">
+        <f>-ItemStatCost!W4</f>
+        <v>-32</v>
+      </c>
+      <c r="C4">
+        <f>POWER(2,ItemStatCost!V4)-ItemStatCost!W4</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5">
+        <f>-ItemStatCost!W5</f>
+        <v>-32</v>
+      </c>
+      <c r="C5">
+        <f>POWER(2,ItemStatCost!V5)-ItemStatCost!W5</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6">
+        <f>-ItemStatCost!W6</f>
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <f>POWER(2,ItemStatCost!V6)-ItemStatCost!W6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7">
+        <f>-ItemStatCost!W7</f>
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <f>POWER(2,ItemStatCost!V7)-ItemStatCost!W7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8">
+        <f>-ItemStatCost!W8</f>
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <f>POWER(2,ItemStatCost!V8)-ItemStatCost!W8</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9">
+        <f>-ItemStatCost!W9</f>
+        <v>-32</v>
+      </c>
+      <c r="C9">
+        <f>POWER(2,ItemStatCost!V9)-ItemStatCost!W9</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10">
+        <f>-ItemStatCost!W10</f>
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <f>POWER(2,ItemStatCost!V10)-ItemStatCost!W10</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11">
+        <f>-ItemStatCost!W11</f>
+        <v>-32</v>
+      </c>
+      <c r="C11">
+        <f>POWER(2,ItemStatCost!V11)-ItemStatCost!W11</f>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12">
+        <f>-ItemStatCost!W12</f>
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <f>POWER(2,ItemStatCost!V12)-ItemStatCost!W12</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13">
+        <f>-ItemStatCost!W13</f>
+        <v>-32</v>
+      </c>
+      <c r="C13">
+        <f>POWER(2,ItemStatCost!V13)-ItemStatCost!W13</f>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14">
+        <f>-ItemStatCost!W14</f>
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <f>POWER(2,ItemStatCost!V14)-ItemStatCost!W14</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15">
+        <f>-ItemStatCost!W15</f>
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <f>POWER(2,ItemStatCost!V15)-ItemStatCost!W15</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16">
+        <f>-ItemStatCost!W16</f>
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <f>POWER(2,ItemStatCost!V16)-ItemStatCost!W16</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17">
+        <f>-ItemStatCost!W17</f>
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <f>POWER(2,ItemStatCost!V17)-ItemStatCost!W17</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18">
+        <f>-ItemStatCost!W18</f>
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <f>POWER(2,ItemStatCost!V18)-ItemStatCost!W18</f>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19">
+        <f>-ItemStatCost!W19</f>
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <f>POWER(2,ItemStatCost!V19)-ItemStatCost!W19</f>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20">
+        <f>-ItemStatCost!W20</f>
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <f>POWER(2,ItemStatCost!V20)-ItemStatCost!W20</f>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21">
+        <f>-ItemStatCost!W21</f>
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <f>POWER(2,ItemStatCost!V21)-ItemStatCost!W21</f>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22">
+        <f>-ItemStatCost!W22</f>
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <f>POWER(2,ItemStatCost!V22)-ItemStatCost!W22</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23">
+        <f>-ItemStatCost!W23</f>
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <f>POWER(2,ItemStatCost!V23)-ItemStatCost!W23</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24">
+        <f>-ItemStatCost!W24</f>
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <f>POWER(2,ItemStatCost!V24)-ItemStatCost!W24</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25">
+        <f>-ItemStatCost!W25</f>
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <f>POWER(2,ItemStatCost!V25)-ItemStatCost!W25</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26">
+        <f>-ItemStatCost!W26</f>
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <f>POWER(2,ItemStatCost!V26)-ItemStatCost!W26</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27">
+        <f>-ItemStatCost!W27</f>
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <f>POWER(2,ItemStatCost!V27)-ItemStatCost!W27</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28">
+        <f>-ItemStatCost!W28</f>
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <f>POWER(2,ItemStatCost!V28)-ItemStatCost!W28</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29">
+        <f>-ItemStatCost!W29</f>
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <f>POWER(2,ItemStatCost!V29)-ItemStatCost!W29</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30">
+        <f>-ItemStatCost!W30</f>
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <f>POWER(2,ItemStatCost!V30)-ItemStatCost!W30</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31">
+        <f>-ItemStatCost!W31</f>
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <f>POWER(2,ItemStatCost!V31)-ItemStatCost!W31</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32">
+        <f>-ItemStatCost!W32</f>
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <f>POWER(2,ItemStatCost!V32)-ItemStatCost!W32</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33">
+        <f>-ItemStatCost!W33</f>
+        <v>-10</v>
+      </c>
+      <c r="C33">
+        <f>POWER(2,ItemStatCost!V33)-ItemStatCost!W33</f>
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34">
+        <f>-ItemStatCost!W34</f>
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <f>POWER(2,ItemStatCost!V34)-ItemStatCost!W34</f>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35">
+        <f>-ItemStatCost!W35</f>
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <f>POWER(2,ItemStatCost!V35)-ItemStatCost!W35</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36">
+        <f>-ItemStatCost!W36</f>
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <f>POWER(2,ItemStatCost!V36)-ItemStatCost!W36</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37">
+        <f>-ItemStatCost!W37</f>
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <f>POWER(2,ItemStatCost!V37)-ItemStatCost!W37</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38">
+        <f>-ItemStatCost!W38</f>
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <f>POWER(2,ItemStatCost!V38)-ItemStatCost!W38</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39">
+        <f>-ItemStatCost!W39</f>
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <f>POWER(2,ItemStatCost!V39)-ItemStatCost!W39</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>116</v>
+      </c>
+      <c r="B40">
+        <f>-ItemStatCost!W40</f>
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <f>POWER(2,ItemStatCost!V40)-ItemStatCost!W40</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41">
+        <f>-ItemStatCost!W41</f>
+        <v>-50</v>
+      </c>
+      <c r="C41">
+        <f>POWER(2,ItemStatCost!V41)-ItemStatCost!W41</f>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>121</v>
+      </c>
+      <c r="B42">
+        <f>-ItemStatCost!W42</f>
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <f>POWER(2,ItemStatCost!V42)-ItemStatCost!W42</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>123</v>
+      </c>
+      <c r="B43">
+        <f>-ItemStatCost!W43</f>
+        <v>-50</v>
+      </c>
+      <c r="C43">
+        <f>POWER(2,ItemStatCost!V43)-ItemStatCost!W43</f>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>125</v>
+      </c>
+      <c r="B44">
+        <f>-ItemStatCost!W44</f>
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <f>POWER(2,ItemStatCost!V44)-ItemStatCost!W44</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>127</v>
+      </c>
+      <c r="B45">
+        <f>-ItemStatCost!W45</f>
+        <v>-50</v>
+      </c>
+      <c r="C45">
+        <f>POWER(2,ItemStatCost!V45)-ItemStatCost!W45</f>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>129</v>
+      </c>
+      <c r="B46">
+        <f>-ItemStatCost!W46</f>
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <f>POWER(2,ItemStatCost!V46)-ItemStatCost!W46</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>131</v>
+      </c>
+      <c r="B47">
+        <f>-ItemStatCost!W47</f>
+        <v>-50</v>
+      </c>
+      <c r="C47">
+        <f>POWER(2,ItemStatCost!V47)-ItemStatCost!W47</f>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>133</v>
+      </c>
+      <c r="B48">
+        <f>-ItemStatCost!W48</f>
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <f>POWER(2,ItemStatCost!V48)-ItemStatCost!W48</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>135</v>
+      </c>
+      <c r="B49">
+        <f>-ItemStatCost!W49</f>
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <f>POWER(2,ItemStatCost!V49)-ItemStatCost!W49</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>136</v>
+      </c>
+      <c r="B50">
+        <f>-ItemStatCost!W50</f>
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <f>POWER(2,ItemStatCost!V50)-ItemStatCost!W50</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>138</v>
+      </c>
+      <c r="B51">
+        <f>-ItemStatCost!W51</f>
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <f>POWER(2,ItemStatCost!V51)-ItemStatCost!W51</f>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>140</v>
+      </c>
+      <c r="B52">
+        <f>-ItemStatCost!W52</f>
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <f>POWER(2,ItemStatCost!V52)-ItemStatCost!W52</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>142</v>
+      </c>
+      <c r="B53">
+        <f>-ItemStatCost!W53</f>
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <f>POWER(2,ItemStatCost!V53)-ItemStatCost!W53</f>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>144</v>
+      </c>
+      <c r="B54">
+        <f>-ItemStatCost!W54</f>
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <f>POWER(2,ItemStatCost!V54)-ItemStatCost!W54</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>146</v>
+      </c>
+      <c r="B55">
+        <f>-ItemStatCost!W55</f>
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <f>POWER(2,ItemStatCost!V55)-ItemStatCost!W55</f>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>147</v>
+      </c>
+      <c r="B56">
+        <f>-ItemStatCost!W56</f>
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <f>POWER(2,ItemStatCost!V56)-ItemStatCost!W56</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>149</v>
+      </c>
+      <c r="B57">
+        <f>-ItemStatCost!W57</f>
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <f>POWER(2,ItemStatCost!V57)-ItemStatCost!W57</f>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>151</v>
+      </c>
+      <c r="B58">
+        <f>-ItemStatCost!W58</f>
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <f>POWER(2,ItemStatCost!V58)-ItemStatCost!W58</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>152</v>
+      </c>
+      <c r="B59">
+        <f>-ItemStatCost!W59</f>
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <f>POWER(2,ItemStatCost!V59)-ItemStatCost!W59</f>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>154</v>
+      </c>
+      <c r="B60">
+        <f>-ItemStatCost!W60</f>
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <f>POWER(2,ItemStatCost!V60)-ItemStatCost!W60</f>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>156</v>
+      </c>
+      <c r="B61">
+        <f>-ItemStatCost!W61</f>
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <f>POWER(2,ItemStatCost!V61)-ItemStatCost!W61</f>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>157</v>
+      </c>
+      <c r="B62">
+        <f>-ItemStatCost!W62</f>
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <f>POWER(2,ItemStatCost!V62)-ItemStatCost!W62</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>159</v>
+      </c>
+      <c r="B63">
+        <f>-ItemStatCost!W63</f>
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <f>POWER(2,ItemStatCost!V63)-ItemStatCost!W63</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>160</v>
+      </c>
+      <c r="B64">
+        <f>-ItemStatCost!W64</f>
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <f>POWER(2,ItemStatCost!V64)-ItemStatCost!W64</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>162</v>
+      </c>
+      <c r="B65">
+        <f>-ItemStatCost!W65</f>
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <f>POWER(2,ItemStatCost!V65)-ItemStatCost!W65</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>163</v>
+      </c>
+      <c r="B66">
+        <f>-ItemStatCost!W66</f>
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <f>POWER(2,ItemStatCost!V66)-ItemStatCost!W66</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>164</v>
+      </c>
+      <c r="B67">
+        <f>-ItemStatCost!W67</f>
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <f>POWER(2,ItemStatCost!V67)-ItemStatCost!W67</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>165</v>
+      </c>
+      <c r="B68">
+        <f>-ItemStatCost!W68</f>
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <f>POWER(2,ItemStatCost!V68)-ItemStatCost!W68</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>166</v>
+      </c>
+      <c r="B69">
+        <f>-ItemStatCost!W69</f>
+        <v>-30</v>
+      </c>
+      <c r="C69">
+        <f>POWER(2,ItemStatCost!V69)-ItemStatCost!W69</f>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>167</v>
+      </c>
+      <c r="B70">
+        <f>-ItemStatCost!W70</f>
+        <v>-30</v>
+      </c>
+      <c r="C70">
+        <f>POWER(2,ItemStatCost!V70)-ItemStatCost!W70</f>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>168</v>
+      </c>
+      <c r="B71">
+        <f>-ItemStatCost!W71</f>
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <f>POWER(2,ItemStatCost!V71)-ItemStatCost!W71</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>169</v>
+      </c>
+      <c r="B72">
+        <f>-ItemStatCost!W72</f>
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <f>POWER(2,ItemStatCost!V72)-ItemStatCost!W72</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>170</v>
+      </c>
+      <c r="B73">
+        <f>-ItemStatCost!W73</f>
+        <v>-100</v>
+      </c>
+      <c r="C73">
+        <f>POWER(2,ItemStatCost!V73)-ItemStatCost!W73</f>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>171</v>
+      </c>
+      <c r="B74">
+        <f>-ItemStatCost!W74</f>
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <f>POWER(2,ItemStatCost!V74)-ItemStatCost!W74</f>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>172</v>
+      </c>
+      <c r="B75">
+        <f>-ItemStatCost!W75</f>
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <f>POWER(2,ItemStatCost!V75)-ItemStatCost!W75</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>173</v>
+      </c>
+      <c r="B76">
+        <f>-ItemStatCost!W76</f>
+        <v>-30</v>
+      </c>
+      <c r="C76">
+        <f>POWER(2,ItemStatCost!V76)-ItemStatCost!W76</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>176</v>
+      </c>
+      <c r="B77">
+        <f>-ItemStatCost!W77</f>
+        <v>-20</v>
+      </c>
+      <c r="C77">
+        <f>POWER(2,ItemStatCost!V77)-ItemStatCost!W77</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>178</v>
+      </c>
+      <c r="B78">
+        <f>-ItemStatCost!W78</f>
+        <v>-10</v>
+      </c>
+      <c r="C78">
+        <f>POWER(2,ItemStatCost!V78)-ItemStatCost!W78</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>180</v>
+      </c>
+      <c r="B79">
+        <f>-ItemStatCost!W79</f>
+        <v>-10</v>
+      </c>
+      <c r="C79">
+        <f>POWER(2,ItemStatCost!V79)-ItemStatCost!W79</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>182</v>
+      </c>
+      <c r="B80">
+        <f>-ItemStatCost!W80</f>
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <f>POWER(2,ItemStatCost!V80)-ItemStatCost!W80</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>185</v>
+      </c>
+      <c r="B81">
+        <f>-ItemStatCost!W81</f>
+        <v>-100</v>
+      </c>
+      <c r="C81">
+        <f>POWER(2,ItemStatCost!V81)-ItemStatCost!W81</f>
+        <v>412</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>187</v>
+      </c>
+      <c r="B82">
+        <f>-ItemStatCost!W82</f>
+        <v>-100</v>
+      </c>
+      <c r="C82">
+        <f>POWER(2,ItemStatCost!V82)-ItemStatCost!W82</f>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>189</v>
+      </c>
+      <c r="B83">
+        <f>-ItemStatCost!W83</f>
+        <v>0</v>
+      </c>
+      <c r="C83">
+        <f>POWER(2,ItemStatCost!V83)-ItemStatCost!W83</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>193</v>
+      </c>
+      <c r="B84">
+        <f>-ItemStatCost!W84</f>
+        <v>-20</v>
+      </c>
+      <c r="C84">
+        <f>POWER(2,ItemStatCost!V84)-ItemStatCost!W84</f>
+        <v>492</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>194</v>
+      </c>
+      <c r="B85">
+        <f>-ItemStatCost!W85</f>
+        <v>0</v>
+      </c>
+      <c r="C85">
+        <f>POWER(2,ItemStatCost!V85)-ItemStatCost!W85</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>196</v>
+      </c>
+      <c r="B86">
+        <f>-ItemStatCost!W86</f>
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <f>POWER(2,ItemStatCost!V86)-ItemStatCost!W86</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>197</v>
+      </c>
+      <c r="B87">
+        <f>-ItemStatCost!W87</f>
+        <v>-50</v>
+      </c>
+      <c r="C87">
+        <f>POWER(2,ItemStatCost!V87)-ItemStatCost!W87</f>
+        <v>462</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>199</v>
+      </c>
+      <c r="B88">
+        <f>-ItemStatCost!W88</f>
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <f>POWER(2,ItemStatCost!V88)-ItemStatCost!W88</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>202</v>
+      </c>
+      <c r="B89">
+        <f>-ItemStatCost!W89</f>
+        <v>0</v>
+      </c>
+      <c r="C89">
+        <f>POWER(2,ItemStatCost!V89)-ItemStatCost!W89</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>204</v>
+      </c>
+      <c r="B90">
+        <f>-ItemStatCost!W90</f>
+        <v>0</v>
+      </c>
+      <c r="C90">
+        <f>POWER(2,ItemStatCost!V90)-ItemStatCost!W90</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>205</v>
+      </c>
+      <c r="B91">
+        <f>-ItemStatCost!W91</f>
+        <v>-4</v>
+      </c>
+      <c r="C91">
+        <f>POWER(2,ItemStatCost!V91)-ItemStatCost!W91</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>207</v>
+      </c>
+      <c r="B92">
+        <f>-ItemStatCost!W92</f>
+        <v>0</v>
+      </c>
+      <c r="C92">
+        <f>POWER(2,ItemStatCost!V92)-ItemStatCost!W92</f>
+        <v>16777216</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>208</v>
+      </c>
+      <c r="B93">
+        <f>-ItemStatCost!W93</f>
+        <v>-100</v>
+      </c>
+      <c r="C93">
+        <f>POWER(2,ItemStatCost!V93)-ItemStatCost!W93</f>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>210</v>
+      </c>
+      <c r="B94">
+        <f>-ItemStatCost!W94</f>
+        <v>0</v>
+      </c>
+      <c r="C94">
+        <f>POWER(2,ItemStatCost!V94)-ItemStatCost!W94</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>211</v>
+      </c>
+      <c r="B95">
+        <f>-ItemStatCost!W95</f>
+        <v>-20</v>
+      </c>
+      <c r="C95">
+        <f>POWER(2,ItemStatCost!V95)-ItemStatCost!W95</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>213</v>
+      </c>
+      <c r="B96">
+        <f>-ItemStatCost!W96</f>
+        <v>-64</v>
+      </c>
+      <c r="C96">
+        <f>POWER(2,ItemStatCost!V96)-ItemStatCost!W96</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>214</v>
+      </c>
+      <c r="B97">
+        <f>-ItemStatCost!W97</f>
+        <v>0</v>
+      </c>
+      <c r="C97">
+        <f>POWER(2,ItemStatCost!V97)-ItemStatCost!W97</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>215</v>
+      </c>
+      <c r="B98">
+        <f>-ItemStatCost!W98</f>
+        <v>-20</v>
+      </c>
+      <c r="C98">
+        <f>POWER(2,ItemStatCost!V98)-ItemStatCost!W98</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>217</v>
+      </c>
+      <c r="B99">
+        <f>-ItemStatCost!W99</f>
+        <v>0</v>
+      </c>
+      <c r="C99">
+        <f>POWER(2,ItemStatCost!V99)-ItemStatCost!W99</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>218</v>
+      </c>
+      <c r="B100">
+        <f>-ItemStatCost!W100</f>
+        <v>0</v>
+      </c>
+      <c r="C100">
+        <f>POWER(2,ItemStatCost!V100)-ItemStatCost!W100</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>219</v>
+      </c>
+      <c r="B101">
+        <f>-ItemStatCost!W101</f>
+        <v>-20</v>
+      </c>
+      <c r="C101">
+        <f>POWER(2,ItemStatCost!V101)-ItemStatCost!W101</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>221</v>
+      </c>
+      <c r="B102">
+        <f>-ItemStatCost!W102</f>
+        <v>0</v>
+      </c>
+      <c r="C102">
+        <f>POWER(2,ItemStatCost!V102)-ItemStatCost!W102</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>222</v>
+      </c>
+      <c r="B103">
+        <f>-ItemStatCost!W103</f>
+        <v>0</v>
+      </c>
+      <c r="C103">
+        <f>POWER(2,ItemStatCost!V103)-ItemStatCost!W103</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>223</v>
+      </c>
+      <c r="B104">
+        <f>-ItemStatCost!W104</f>
+        <v>-20</v>
+      </c>
+      <c r="C104">
+        <f>POWER(2,ItemStatCost!V104)-ItemStatCost!W104</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>225</v>
+      </c>
+      <c r="B105">
+        <f>-ItemStatCost!W105</f>
+        <v>0</v>
+      </c>
+      <c r="C105">
+        <f>POWER(2,ItemStatCost!V105)-ItemStatCost!W105</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>226</v>
+      </c>
+      <c r="B106">
+        <f>-ItemStatCost!W106</f>
+        <v>0</v>
+      </c>
+      <c r="C106">
+        <f>POWER(2,ItemStatCost!V106)-ItemStatCost!W106</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>227</v>
+      </c>
+      <c r="B107">
+        <f>-ItemStatCost!W107</f>
+        <v>-20</v>
+      </c>
+      <c r="C107">
+        <f>POWER(2,ItemStatCost!V107)-ItemStatCost!W107</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>229</v>
+      </c>
+      <c r="B108">
+        <f>-ItemStatCost!W108</f>
+        <v>0</v>
+      </c>
+      <c r="C108">
+        <f>POWER(2,ItemStatCost!V108)-ItemStatCost!W108</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>230</v>
+      </c>
+      <c r="B109">
+        <f>-ItemStatCost!W109</f>
+        <v>0</v>
+      </c>
+      <c r="C109">
+        <f>POWER(2,ItemStatCost!V109)-ItemStatCost!W109</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>231</v>
+      </c>
+      <c r="B110">
+        <f>-ItemStatCost!W110</f>
+        <v>0</v>
+      </c>
+      <c r="C110">
+        <f>POWER(2,ItemStatCost!V110)-ItemStatCost!W110</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>233</v>
+      </c>
+      <c r="B111">
+        <f>-ItemStatCost!W111</f>
+        <v>0</v>
+      </c>
+      <c r="C111">
+        <f>POWER(2,ItemStatCost!V111)-ItemStatCost!W111</f>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>234</v>
+      </c>
+      <c r="B112">
+        <f>-ItemStatCost!W112</f>
+        <v>-20</v>
+      </c>
+      <c r="C112">
+        <f>POWER(2,ItemStatCost!V112)-ItemStatCost!W112</f>
+        <v>236</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>236</v>
+      </c>
+      <c r="B113">
+        <f>-ItemStatCost!W113</f>
+        <v>-20</v>
+      </c>
+      <c r="C113">
+        <f>POWER(2,ItemStatCost!V113)-ItemStatCost!W113</f>
+        <v>492</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>238</v>
+      </c>
+      <c r="B114">
+        <f>-ItemStatCost!W114</f>
+        <v>1</v>
+      </c>
+      <c r="C114">
+        <f>POWER(2,ItemStatCost!V114)-ItemStatCost!W114</f>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>240</v>
+      </c>
+      <c r="B115">
+        <f>-ItemStatCost!W115</f>
+        <v>0</v>
+      </c>
+      <c r="C115">
+        <f>POWER(2,ItemStatCost!V115)-ItemStatCost!W115</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>242</v>
+      </c>
+      <c r="B116">
+        <f>-ItemStatCost!W116</f>
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <f>POWER(2,ItemStatCost!V116)-ItemStatCost!W116</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>245</v>
+      </c>
+      <c r="B117">
+        <f>-ItemStatCost!W117</f>
+        <v>0</v>
+      </c>
+      <c r="C117">
+        <f>POWER(2,ItemStatCost!V117)-ItemStatCost!W117</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>247</v>
+      </c>
+      <c r="B118">
+        <f>-ItemStatCost!W118</f>
+        <v>0</v>
+      </c>
+      <c r="C118">
+        <f>POWER(2,ItemStatCost!V118)-ItemStatCost!W118</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>249</v>
+      </c>
+      <c r="B119">
+        <f>-ItemStatCost!W119</f>
+        <v>0</v>
+      </c>
+      <c r="C119">
+        <f>POWER(2,ItemStatCost!V119)-ItemStatCost!W119</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>251</v>
+      </c>
+      <c r="B120">
+        <f>-ItemStatCost!W120</f>
+        <v>0</v>
+      </c>
+      <c r="C120">
+        <f>POWER(2,ItemStatCost!V120)-ItemStatCost!W120</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>253</v>
+      </c>
+      <c r="B121">
+        <f>-ItemStatCost!W121</f>
+        <v>-20</v>
+      </c>
+      <c r="C121">
+        <f>POWER(2,ItemStatCost!V121)-ItemStatCost!W121</f>
+        <v>492</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>255</v>
+      </c>
+      <c r="B122">
+        <f>-ItemStatCost!W122</f>
+        <v>-128</v>
+      </c>
+      <c r="C122">
+        <f>POWER(2,ItemStatCost!V122)-ItemStatCost!W122</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>257</v>
+      </c>
+      <c r="B123">
+        <f>-ItemStatCost!W123</f>
+        <v>-20</v>
+      </c>
+      <c r="C123">
+        <f>POWER(2,ItemStatCost!V123)-ItemStatCost!W123</f>
+        <v>492</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>259</v>
+      </c>
+      <c r="B124">
+        <f>-ItemStatCost!W124</f>
+        <v>-20</v>
+      </c>
+      <c r="C124">
+        <f>POWER(2,ItemStatCost!V124)-ItemStatCost!W124</f>
+        <v>492</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>261</v>
+      </c>
+      <c r="B125">
+        <f>-ItemStatCost!W125</f>
+        <v>-128</v>
+      </c>
+      <c r="C125">
+        <f>POWER(2,ItemStatCost!V125)-ItemStatCost!W125</f>
+        <v>896</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>263</v>
+      </c>
+      <c r="B126">
+        <f>-ItemStatCost!W126</f>
+        <v>-128</v>
+      </c>
+      <c r="C126">
+        <f>POWER(2,ItemStatCost!V126)-ItemStatCost!W126</f>
+        <v>896</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>265</v>
+      </c>
+      <c r="B127">
+        <f>-ItemStatCost!W127</f>
+        <v>0</v>
+      </c>
+      <c r="C127">
+        <f>POWER(2,ItemStatCost!V127)-ItemStatCost!W127</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>267</v>
+      </c>
+      <c r="B128">
+        <f>-ItemStatCost!W128</f>
+        <v>0</v>
+      </c>
+      <c r="C128">
+        <f>POWER(2,ItemStatCost!V128)-ItemStatCost!W128</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>269</v>
+      </c>
+      <c r="B129">
+        <f>-ItemStatCost!W129</f>
+        <v>0</v>
+      </c>
+      <c r="C129">
+        <f>POWER(2,ItemStatCost!V129)-ItemStatCost!W129</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>271</v>
+      </c>
+      <c r="B130">
+        <f>-ItemStatCost!W130</f>
+        <v>0</v>
+      </c>
+      <c r="C130">
+        <f>POWER(2,ItemStatCost!V130)-ItemStatCost!W130</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>273</v>
+      </c>
+      <c r="B131">
+        <f>-ItemStatCost!W131</f>
+        <v>0</v>
+      </c>
+      <c r="C131">
+        <f>POWER(2,ItemStatCost!V131)-ItemStatCost!W131</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>274</v>
+      </c>
+      <c r="B132">
+        <f>-ItemStatCost!W132</f>
+        <v>0</v>
+      </c>
+      <c r="C132">
+        <f>POWER(2,ItemStatCost!V132)-ItemStatCost!W132</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>275</v>
+      </c>
+      <c r="B133">
+        <f>-ItemStatCost!W133</f>
+        <v>0</v>
+      </c>
+      <c r="C133">
+        <f>POWER(2,ItemStatCost!V133)-ItemStatCost!W133</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>276</v>
+      </c>
+      <c r="B134">
+        <f>-ItemStatCost!W134</f>
+        <v>0</v>
+      </c>
+      <c r="C134">
+        <f>POWER(2,ItemStatCost!V134)-ItemStatCost!W134</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>277</v>
+      </c>
+      <c r="B135">
+        <f>-ItemStatCost!W135</f>
+        <v>0</v>
+      </c>
+      <c r="C135">
+        <f>POWER(2,ItemStatCost!V135)-ItemStatCost!W135</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>278</v>
+      </c>
+      <c r="B136">
+        <f>-ItemStatCost!W136</f>
+        <v>0</v>
+      </c>
+      <c r="C136">
+        <f>POWER(2,ItemStatCost!V136)-ItemStatCost!W136</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>280</v>
+      </c>
+      <c r="B137">
+        <f>-ItemStatCost!W137</f>
+        <v>0</v>
+      </c>
+      <c r="C137">
+        <f>POWER(2,ItemStatCost!V137)-ItemStatCost!W137</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>282</v>
+      </c>
+      <c r="B138">
+        <f>-ItemStatCost!W138</f>
+        <v>0</v>
+      </c>
+      <c r="C138">
+        <f>POWER(2,ItemStatCost!V138)-ItemStatCost!W138</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>284</v>
+      </c>
+      <c r="B139">
+        <f>-ItemStatCost!W139</f>
+        <v>0</v>
+      </c>
+      <c r="C139">
+        <f>POWER(2,ItemStatCost!V139)-ItemStatCost!W139</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>286</v>
+      </c>
+      <c r="B140">
+        <f>-ItemStatCost!W140</f>
+        <v>0</v>
+      </c>
+      <c r="C140">
+        <f>POWER(2,ItemStatCost!V140)-ItemStatCost!W140</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>288</v>
+      </c>
+      <c r="B141">
+        <f>-ItemStatCost!W141</f>
+        <v>0</v>
+      </c>
+      <c r="C141">
+        <f>POWER(2,ItemStatCost!V141)-ItemStatCost!W141</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>290</v>
+      </c>
+      <c r="B142">
+        <f>-ItemStatCost!W142</f>
+        <v>0</v>
+      </c>
+      <c r="C142">
+        <f>POWER(2,ItemStatCost!V142)-ItemStatCost!W142</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>291</v>
+      </c>
+      <c r="B143">
+        <f>-ItemStatCost!W143</f>
+        <v>0</v>
+      </c>
+      <c r="C143">
+        <f>POWER(2,ItemStatCost!V143)-ItemStatCost!W143</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>293</v>
+      </c>
+      <c r="B144">
+        <f>-ItemStatCost!W144</f>
+        <v>0</v>
+      </c>
+      <c r="C144">
+        <f>POWER(2,ItemStatCost!V144)-ItemStatCost!W144</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>295</v>
+      </c>
+      <c r="B145">
+        <f>-ItemStatCost!W145</f>
+        <v>0</v>
+      </c>
+      <c r="C145">
+        <f>POWER(2,ItemStatCost!V145)-ItemStatCost!W145</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>297</v>
+      </c>
+      <c r="B146">
+        <f>-ItemStatCost!W146</f>
+        <v>0</v>
+      </c>
+      <c r="C146">
+        <f>POWER(2,ItemStatCost!V146)-ItemStatCost!W146</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>299</v>
+      </c>
+      <c r="B147">
+        <f>-ItemStatCost!W147</f>
+        <v>0</v>
+      </c>
+      <c r="C147">
+        <f>POWER(2,ItemStatCost!V147)-ItemStatCost!W147</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>301</v>
+      </c>
+      <c r="B148">
+        <f>-ItemStatCost!W148</f>
+        <v>0</v>
+      </c>
+      <c r="C148">
+        <f>POWER(2,ItemStatCost!V148)-ItemStatCost!W148</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>303</v>
+      </c>
+      <c r="B149">
+        <f>-ItemStatCost!W149</f>
+        <v>0</v>
+      </c>
+      <c r="C149">
+        <f>POWER(2,ItemStatCost!V149)-ItemStatCost!W149</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>305</v>
+      </c>
+      <c r="B150">
+        <f>-ItemStatCost!W150</f>
+        <v>0</v>
+      </c>
+      <c r="C150">
+        <f>POWER(2,ItemStatCost!V150)-ItemStatCost!W150</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>307</v>
+      </c>
+      <c r="B151">
+        <f>-ItemStatCost!W151</f>
+        <v>0</v>
+      </c>
+      <c r="C151">
+        <f>POWER(2,ItemStatCost!V151)-ItemStatCost!W151</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>309</v>
+      </c>
+      <c r="B152">
+        <f>-ItemStatCost!W152</f>
+        <v>0</v>
+      </c>
+      <c r="C152">
+        <f>POWER(2,ItemStatCost!V152)-ItemStatCost!W152</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>311</v>
+      </c>
+      <c r="B153">
+        <f>-ItemStatCost!W153</f>
+        <v>0</v>
+      </c>
+      <c r="C153">
+        <f>POWER(2,ItemStatCost!V153)-ItemStatCost!W153</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>313</v>
+      </c>
+      <c r="B154">
+        <f>-ItemStatCost!W154</f>
+        <v>0</v>
+      </c>
+      <c r="C154">
+        <f>POWER(2,ItemStatCost!V154)-ItemStatCost!W154</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>315</v>
+      </c>
+      <c r="B155">
+        <f>-ItemStatCost!W155</f>
+        <v>0</v>
+      </c>
+      <c r="C155">
+        <f>POWER(2,ItemStatCost!V155)-ItemStatCost!W155</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>317</v>
+      </c>
+      <c r="B156">
+        <f>-ItemStatCost!W156</f>
+        <v>-20</v>
+      </c>
+      <c r="C156">
+        <f>POWER(2,ItemStatCost!V156)-ItemStatCost!W156</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>319</v>
+      </c>
+      <c r="B157">
+        <f>-ItemStatCost!W157</f>
+        <v>0</v>
+      </c>
+      <c r="C157">
+        <f>POWER(2,ItemStatCost!V157)-ItemStatCost!W157</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>321</v>
+      </c>
+      <c r="B158">
+        <f>-ItemStatCost!W158</f>
+        <v>0</v>
+      </c>
+      <c r="C158">
+        <f>POWER(2,ItemStatCost!V158)-ItemStatCost!W158</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>323</v>
+      </c>
+      <c r="B159">
+        <f>-ItemStatCost!W159</f>
+        <v>0</v>
+      </c>
+      <c r="C159">
+        <f>POWER(2,ItemStatCost!V159)-ItemStatCost!W159</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>325</v>
+      </c>
+      <c r="B160">
+        <f>-ItemStatCost!W160</f>
+        <v>0</v>
+      </c>
+      <c r="C160">
+        <f>POWER(2,ItemStatCost!V160)-ItemStatCost!W160</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>88</v>
+      </c>
+      <c r="B161">
+        <f>-ItemStatCost!W161</f>
+        <v>0</v>
+      </c>
+      <c r="C161">
+        <f>POWER(2,ItemStatCost!V161)-ItemStatCost!W161</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>83</v>
+      </c>
+      <c r="B162">
+        <f>-ItemStatCost!W162</f>
+        <v>0</v>
+      </c>
+      <c r="C162">
+        <f>POWER(2,ItemStatCost!V162)-ItemStatCost!W162</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>327</v>
+      </c>
+      <c r="B163">
+        <f>-ItemStatCost!W163</f>
+        <v>0</v>
+      </c>
+      <c r="C163">
+        <f>POWER(2,ItemStatCost!V163)-ItemStatCost!W163</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>328</v>
+      </c>
+      <c r="B164">
+        <f>-ItemStatCost!W164</f>
+        <v>0</v>
+      </c>
+      <c r="C164">
+        <f>POWER(2,ItemStatCost!V164)-ItemStatCost!W164</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>329</v>
+      </c>
+      <c r="B165">
+        <f>-ItemStatCost!W165</f>
+        <v>0</v>
+      </c>
+      <c r="C165">
+        <f>POWER(2,ItemStatCost!V165)-ItemStatCost!W165</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>330</v>
+      </c>
+      <c r="B166">
+        <f>-ItemStatCost!W166</f>
+        <v>0</v>
+      </c>
+      <c r="C166">
+        <f>POWER(2,ItemStatCost!V166)-ItemStatCost!W166</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>331</v>
+      </c>
+      <c r="B167">
+        <f>-ItemStatCost!W167</f>
+        <v>0</v>
+      </c>
+      <c r="C167">
+        <f>POWER(2,ItemStatCost!V167)-ItemStatCost!W167</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>332</v>
+      </c>
+      <c r="B168">
+        <f>-ItemStatCost!W168</f>
+        <v>0</v>
+      </c>
+      <c r="C168">
+        <f>POWER(2,ItemStatCost!V168)-ItemStatCost!W168</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>333</v>
+      </c>
+      <c r="B169">
+        <f>-ItemStatCost!W169</f>
+        <v>0</v>
+      </c>
+      <c r="C169">
+        <f>POWER(2,ItemStatCost!V169)-ItemStatCost!W169</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>334</v>
+      </c>
+      <c r="B170">
+        <f>-ItemStatCost!W170</f>
+        <v>0</v>
+      </c>
+      <c r="C170">
+        <f>POWER(2,ItemStatCost!V170)-ItemStatCost!W170</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>335</v>
+      </c>
+      <c r="B171">
+        <f>-ItemStatCost!W171</f>
+        <v>0</v>
+      </c>
+      <c r="C171">
+        <f>POWER(2,ItemStatCost!V171)-ItemStatCost!W171</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>336</v>
+      </c>
+      <c r="B172">
+        <f>-ItemStatCost!W172</f>
+        <v>0</v>
+      </c>
+      <c r="C172">
+        <f>POWER(2,ItemStatCost!V172)-ItemStatCost!W172</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>337</v>
+      </c>
+      <c r="B173">
+        <f>-ItemStatCost!W173</f>
+        <v>0</v>
+      </c>
+      <c r="C173">
+        <f>POWER(2,ItemStatCost!V173)-ItemStatCost!W173</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>338</v>
+      </c>
+      <c r="B174">
+        <f>-ItemStatCost!W174</f>
+        <v>0</v>
+      </c>
+      <c r="C174">
+        <f>POWER(2,ItemStatCost!V174)-ItemStatCost!W174</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>339</v>
+      </c>
+      <c r="B175">
+        <f>-ItemStatCost!W175</f>
+        <v>0</v>
+      </c>
+      <c r="C175">
+        <f>POWER(2,ItemStatCost!V175)-ItemStatCost!W175</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>340</v>
+      </c>
+      <c r="B176">
+        <f>-ItemStatCost!W176</f>
+        <v>0</v>
+      </c>
+      <c r="C176">
+        <f>POWER(2,ItemStatCost!V176)-ItemStatCost!W176</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>341</v>
+      </c>
+      <c r="B177">
+        <f>-ItemStatCost!W177</f>
+        <v>0</v>
+      </c>
+      <c r="C177">
+        <f>POWER(2,ItemStatCost!V177)-ItemStatCost!W177</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>342</v>
+      </c>
+      <c r="B178">
+        <f>-ItemStatCost!W178</f>
+        <v>0</v>
+      </c>
+      <c r="C178">
+        <f>POWER(2,ItemStatCost!V178)-ItemStatCost!W178</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>343</v>
+      </c>
+      <c r="B179">
+        <f>-ItemStatCost!W179</f>
+        <v>0</v>
+      </c>
+      <c r="C179">
+        <f>POWER(2,ItemStatCost!V179)-ItemStatCost!W179</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>344</v>
+      </c>
+      <c r="B180">
+        <f>-ItemStatCost!W180</f>
+        <v>0</v>
+      </c>
+      <c r="C180">
+        <f>POWER(2,ItemStatCost!V180)-ItemStatCost!W180</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>345</v>
+      </c>
+      <c r="B181">
+        <f>-ItemStatCost!W181</f>
+        <v>0</v>
+      </c>
+      <c r="C181">
+        <f>POWER(2,ItemStatCost!V181)-ItemStatCost!W181</f>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>347</v>
+      </c>
+      <c r="B182">
+        <f>-ItemStatCost!W182</f>
+        <v>0</v>
+      </c>
+      <c r="C182">
+        <f>POWER(2,ItemStatCost!V182)-ItemStatCost!W182</f>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>349</v>
+      </c>
+      <c r="B183">
+        <f>-ItemStatCost!W183</f>
+        <v>0</v>
+      </c>
+      <c r="C183">
+        <f>POWER(2,ItemStatCost!V183)-ItemStatCost!W183</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>350</v>
+      </c>
+      <c r="B184">
+        <f>-ItemStatCost!W184</f>
+        <v>0</v>
+      </c>
+      <c r="C184">
+        <f>POWER(2,ItemStatCost!V184)-ItemStatCost!W184</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>351</v>
+      </c>
+      <c r="B185">
+        <f>-ItemStatCost!W185</f>
+        <v>0</v>
+      </c>
+      <c r="C185">
+        <f>POWER(2,ItemStatCost!V185)-ItemStatCost!W185</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>352</v>
+      </c>
+      <c r="B186">
+        <f>-ItemStatCost!W186</f>
+        <v>0</v>
+      </c>
+      <c r="C186">
+        <f>POWER(2,ItemStatCost!V186)-ItemStatCost!W186</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>353</v>
+      </c>
+      <c r="B187">
+        <f>-ItemStatCost!W187</f>
+        <v>0</v>
+      </c>
+      <c r="C187">
+        <f>POWER(2,ItemStatCost!V187)-ItemStatCost!W187</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>354</v>
+      </c>
+      <c r="B188">
+        <f>-ItemStatCost!W188</f>
+        <v>0</v>
+      </c>
+      <c r="C188">
+        <f>POWER(2,ItemStatCost!V188)-ItemStatCost!W188</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>355</v>
+      </c>
+      <c r="B189">
+        <f>-ItemStatCost!W189</f>
+        <v>0</v>
+      </c>
+      <c r="C189">
+        <f>POWER(2,ItemStatCost!V189)-ItemStatCost!W189</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>356</v>
+      </c>
+      <c r="B190">
+        <f>-ItemStatCost!W190</f>
+        <v>0</v>
+      </c>
+      <c r="C190">
+        <f>POWER(2,ItemStatCost!V190)-ItemStatCost!W190</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>358</v>
+      </c>
+      <c r="B191">
+        <f>-ItemStatCost!W191</f>
+        <v>0</v>
+      </c>
+      <c r="C191">
+        <f>POWER(2,ItemStatCost!V191)-ItemStatCost!W191</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>359</v>
+      </c>
+      <c r="B192">
+        <f>-ItemStatCost!W192</f>
+        <v>0</v>
+      </c>
+      <c r="C192">
+        <f>POWER(2,ItemStatCost!V192)-ItemStatCost!W192</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>360</v>
+      </c>
+      <c r="B193">
+        <f>-ItemStatCost!W193</f>
+        <v>0</v>
+      </c>
+      <c r="C193">
+        <f>POWER(2,ItemStatCost!V193)-ItemStatCost!W193</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>361</v>
+      </c>
+      <c r="B194">
+        <f>-ItemStatCost!W194</f>
+        <v>0</v>
+      </c>
+      <c r="C194">
+        <f>POWER(2,ItemStatCost!V194)-ItemStatCost!W194</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>362</v>
+      </c>
+      <c r="B195">
+        <f>-ItemStatCost!W195</f>
+        <v>0</v>
+      </c>
+      <c r="C195">
+        <f>POWER(2,ItemStatCost!V195)-ItemStatCost!W195</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>363</v>
+      </c>
+      <c r="B196">
+        <f>-ItemStatCost!W196</f>
+        <v>0</v>
+      </c>
+      <c r="C196">
+        <f>POWER(2,ItemStatCost!V196)-ItemStatCost!W196</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>364</v>
+      </c>
+      <c r="B197">
+        <f>-ItemStatCost!W197</f>
+        <v>0</v>
+      </c>
+      <c r="C197">
+        <f>POWER(2,ItemStatCost!V197)-ItemStatCost!W197</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>368</v>
+      </c>
+      <c r="B198">
+        <f>-ItemStatCost!W198</f>
+        <v>0</v>
+      </c>
+      <c r="C198">
+        <f>POWER(2,ItemStatCost!V198)-ItemStatCost!W198</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>370</v>
+      </c>
+      <c r="B199">
+        <f>-ItemStatCost!W199</f>
+        <v>0</v>
+      </c>
+      <c r="C199">
+        <f>POWER(2,ItemStatCost!V199)-ItemStatCost!W199</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>373</v>
+      </c>
+      <c r="B200">
+        <f>-ItemStatCost!W200</f>
+        <v>0</v>
+      </c>
+      <c r="C200">
+        <f>POWER(2,ItemStatCost!V200)-ItemStatCost!W200</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>375</v>
+      </c>
+      <c r="B201">
+        <f>-ItemStatCost!W201</f>
+        <v>0</v>
+      </c>
+      <c r="C201">
+        <f>POWER(2,ItemStatCost!V201)-ItemStatCost!W201</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>378</v>
+      </c>
+      <c r="B202">
+        <f>-ItemStatCost!W202</f>
+        <v>0</v>
+      </c>
+      <c r="C202">
+        <f>POWER(2,ItemStatCost!V202)-ItemStatCost!W202</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>379</v>
+      </c>
+      <c r="B203">
+        <f>-ItemStatCost!W203</f>
+        <v>0</v>
+      </c>
+      <c r="C203">
+        <f>POWER(2,ItemStatCost!V203)-ItemStatCost!W203</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>381</v>
+      </c>
+      <c r="B204">
+        <f>-ItemStatCost!W204</f>
+        <v>0</v>
+      </c>
+      <c r="C204">
+        <f>POWER(2,ItemStatCost!V204)-ItemStatCost!W204</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>382</v>
+      </c>
+      <c r="B205">
+        <f>-ItemStatCost!W205</f>
+        <v>0</v>
+      </c>
+      <c r="C205">
+        <f>POWER(2,ItemStatCost!V205)-ItemStatCost!W205</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>383</v>
+      </c>
+      <c r="B206">
+        <f>-ItemStatCost!W206</f>
+        <v>0</v>
+      </c>
+      <c r="C206">
+        <f>POWER(2,ItemStatCost!V206)-ItemStatCost!W206</f>
+        <v>65536</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>385</v>
+      </c>
+      <c r="B207">
+        <f>-ItemStatCost!W207</f>
+        <v>0</v>
+      </c>
+      <c r="C207">
+        <f>POWER(2,ItemStatCost!V207)-ItemStatCost!W207</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>386</v>
+      </c>
+      <c r="B208">
+        <f>-ItemStatCost!W208</f>
+        <v>0</v>
+      </c>
+      <c r="C208">
+        <f>POWER(2,ItemStatCost!V208)-ItemStatCost!W208</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>387</v>
+      </c>
+      <c r="B209">
+        <f>-ItemStatCost!W209</f>
+        <v>0</v>
+      </c>
+      <c r="C209">
+        <f>POWER(2,ItemStatCost!V209)-ItemStatCost!W209</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>388</v>
+      </c>
+      <c r="B210">
+        <f>-ItemStatCost!W210</f>
+        <v>0</v>
+      </c>
+      <c r="C210">
+        <f>POWER(2,ItemStatCost!V210)-ItemStatCost!W210</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>389</v>
+      </c>
+      <c r="B211">
+        <f>-ItemStatCost!W211</f>
+        <v>0</v>
+      </c>
+      <c r="C211">
+        <f>POWER(2,ItemStatCost!V211)-ItemStatCost!W211</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>390</v>
+      </c>
+      <c r="B212">
+        <f>-ItemStatCost!W212</f>
+        <v>0</v>
+      </c>
+      <c r="C212">
+        <f>POWER(2,ItemStatCost!V212)-ItemStatCost!W212</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>391</v>
+      </c>
+      <c r="B213">
+        <f>-ItemStatCost!W213</f>
+        <v>0</v>
+      </c>
+      <c r="C213">
+        <f>POWER(2,ItemStatCost!V213)-ItemStatCost!W213</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>392</v>
+      </c>
+      <c r="B214">
+        <f>-ItemStatCost!W214</f>
+        <v>0</v>
+      </c>
+      <c r="C214">
+        <f>POWER(2,ItemStatCost!V214)-ItemStatCost!W214</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>393</v>
+      </c>
+      <c r="B215">
+        <f>-ItemStatCost!W215</f>
+        <v>0</v>
+      </c>
+      <c r="C215">
+        <f>POWER(2,ItemStatCost!V215)-ItemStatCost!W215</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>394</v>
+      </c>
+      <c r="B216">
+        <f>-ItemStatCost!W216</f>
+        <v>0</v>
+      </c>
+      <c r="C216">
+        <f>POWER(2,ItemStatCost!V216)-ItemStatCost!W216</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>396</v>
+      </c>
+      <c r="B217">
+        <f>-ItemStatCost!W217</f>
+        <v>0</v>
+      </c>
+      <c r="C217">
+        <f>POWER(2,ItemStatCost!V217)-ItemStatCost!W217</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>397</v>
+      </c>
+      <c r="B218">
+        <f>-ItemStatCost!W218</f>
+        <v>0</v>
+      </c>
+      <c r="C218">
+        <f>POWER(2,ItemStatCost!V218)-ItemStatCost!W218</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>398</v>
+      </c>
+      <c r="B219">
+        <f>-ItemStatCost!W219</f>
+        <v>0</v>
+      </c>
+      <c r="C219">
+        <f>POWER(2,ItemStatCost!V219)-ItemStatCost!W219</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>399</v>
+      </c>
+      <c r="B220">
+        <f>-ItemStatCost!W220</f>
+        <v>0</v>
+      </c>
+      <c r="C220">
+        <f>POWER(2,ItemStatCost!V220)-ItemStatCost!W220</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>400</v>
+      </c>
+      <c r="B221">
+        <f>-ItemStatCost!W221</f>
+        <v>0</v>
+      </c>
+      <c r="C221">
+        <f>POWER(2,ItemStatCost!V221)-ItemStatCost!W221</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>401</v>
+      </c>
+      <c r="B222">
+        <f>-ItemStatCost!W222</f>
+        <v>0</v>
+      </c>
+      <c r="C222">
+        <f>POWER(2,ItemStatCost!V222)-ItemStatCost!W222</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>402</v>
+      </c>
+      <c r="B223">
+        <f>-ItemStatCost!W223</f>
+        <v>0</v>
+      </c>
+      <c r="C223">
+        <f>POWER(2,ItemStatCost!V223)-ItemStatCost!W223</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>403</v>
+      </c>
+      <c r="B224">
+        <f>-ItemStatCost!W224</f>
+        <v>0</v>
+      </c>
+      <c r="C224">
+        <f>POWER(2,ItemStatCost!V224)-ItemStatCost!W224</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>404</v>
+      </c>
+      <c r="B225">
+        <f>-ItemStatCost!W225</f>
+        <v>0</v>
+      </c>
+      <c r="C225">
+        <f>POWER(2,ItemStatCost!V225)-ItemStatCost!W225</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>405</v>
+      </c>
+      <c r="B226">
+        <f>-ItemStatCost!W226</f>
+        <v>0</v>
+      </c>
+      <c r="C226">
+        <f>POWER(2,ItemStatCost!V226)-ItemStatCost!W226</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>406</v>
+      </c>
+      <c r="B227">
+        <f>-ItemStatCost!W227</f>
+        <v>0</v>
+      </c>
+      <c r="C227">
+        <f>POWER(2,ItemStatCost!V227)-ItemStatCost!W227</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>407</v>
+      </c>
+      <c r="B228">
+        <f>-ItemStatCost!W228</f>
+        <v>0</v>
+      </c>
+      <c r="C228">
+        <f>POWER(2,ItemStatCost!V228)-ItemStatCost!W228</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>408</v>
+      </c>
+      <c r="B229">
+        <f>-ItemStatCost!W229</f>
+        <v>0</v>
+      </c>
+      <c r="C229">
+        <f>POWER(2,ItemStatCost!V229)-ItemStatCost!W229</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>409</v>
+      </c>
+      <c r="B230">
+        <f>-ItemStatCost!W230</f>
+        <v>0</v>
+      </c>
+      <c r="C230">
+        <f>POWER(2,ItemStatCost!V230)-ItemStatCost!W230</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>410</v>
+      </c>
+      <c r="B231">
+        <f>-ItemStatCost!W231</f>
+        <v>0</v>
+      </c>
+      <c r="C231">
+        <f>POWER(2,ItemStatCost!V231)-ItemStatCost!W231</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>411</v>
+      </c>
+      <c r="B232">
+        <f>-ItemStatCost!W232</f>
+        <v>0</v>
+      </c>
+      <c r="C232">
+        <f>POWER(2,ItemStatCost!V232)-ItemStatCost!W232</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>412</v>
+      </c>
+      <c r="B233">
+        <f>-ItemStatCost!W233</f>
+        <v>0</v>
+      </c>
+      <c r="C233">
+        <f>POWER(2,ItemStatCost!V233)-ItemStatCost!W233</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>413</v>
+      </c>
+      <c r="B234">
+        <f>-ItemStatCost!W234</f>
+        <v>0</v>
+      </c>
+      <c r="C234">
+        <f>POWER(2,ItemStatCost!V234)-ItemStatCost!W234</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>414</v>
+      </c>
+      <c r="B235">
+        <f>-ItemStatCost!W235</f>
+        <v>0</v>
+      </c>
+      <c r="C235">
+        <f>POWER(2,ItemStatCost!V235)-ItemStatCost!W235</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>415</v>
+      </c>
+      <c r="B236">
+        <f>-ItemStatCost!W236</f>
+        <v>0</v>
+      </c>
+      <c r="C236">
+        <f>POWER(2,ItemStatCost!V236)-ItemStatCost!W236</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>417</v>
+      </c>
+      <c r="B237">
+        <f>-ItemStatCost!W237</f>
+        <v>0</v>
+      </c>
+      <c r="C237">
+        <f>POWER(2,ItemStatCost!V237)-ItemStatCost!W237</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>419</v>
+      </c>
+      <c r="B238">
+        <f>-ItemStatCost!W238</f>
+        <v>0</v>
+      </c>
+      <c r="C238">
+        <f>POWER(2,ItemStatCost!V238)-ItemStatCost!W238</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>421</v>
+      </c>
+      <c r="B239">
+        <f>-ItemStatCost!W239</f>
+        <v>0</v>
+      </c>
+      <c r="C239">
+        <f>POWER(2,ItemStatCost!V239)-ItemStatCost!W239</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>422</v>
+      </c>
+      <c r="B240">
+        <f>-ItemStatCost!W240</f>
+        <v>0</v>
+      </c>
+      <c r="C240">
+        <f>POWER(2,ItemStatCost!V240)-ItemStatCost!W240</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>423</v>
+      </c>
+      <c r="B241">
+        <f>-ItemStatCost!W241</f>
+        <v>0</v>
+      </c>
+      <c r="C241">
+        <f>POWER(2,ItemStatCost!V241)-ItemStatCost!W241</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>424</v>
+      </c>
+      <c r="B242">
+        <f>-ItemStatCost!W242</f>
+        <v>0</v>
+      </c>
+      <c r="C242">
+        <f>POWER(2,ItemStatCost!V242)-ItemStatCost!W242</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>425</v>
+      </c>
+      <c r="B243">
+        <f>-ItemStatCost!W243</f>
+        <v>0</v>
+      </c>
+      <c r="C243">
+        <f>POWER(2,ItemStatCost!V243)-ItemStatCost!W243</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>426</v>
+      </c>
+      <c r="B244">
+        <f>-ItemStatCost!W244</f>
+        <v>0</v>
+      </c>
+      <c r="C244">
+        <f>POWER(2,ItemStatCost!V244)-ItemStatCost!W244</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>427</v>
+      </c>
+      <c r="B245">
+        <f>-ItemStatCost!W245</f>
+        <v>0</v>
+      </c>
+      <c r="C245">
+        <f>POWER(2,ItemStatCost!V245)-ItemStatCost!W245</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>428</v>
+      </c>
+      <c r="B246">
+        <f>-ItemStatCost!W246</f>
+        <v>0</v>
+      </c>
+      <c r="C246">
+        <f>POWER(2,ItemStatCost!V246)-ItemStatCost!W246</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>429</v>
+      </c>
+      <c r="B247">
+        <f>-ItemStatCost!W247</f>
+        <v>0</v>
+      </c>
+      <c r="C247">
+        <f>POWER(2,ItemStatCost!V247)-ItemStatCost!W247</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>430</v>
+      </c>
+      <c r="B248">
+        <f>-ItemStatCost!W248</f>
+        <v>0</v>
+      </c>
+      <c r="C248">
+        <f>POWER(2,ItemStatCost!V248)-ItemStatCost!W248</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
+        <v>431</v>
+      </c>
+      <c r="B249">
+        <f>-ItemStatCost!W249</f>
+        <v>0</v>
+      </c>
+      <c r="C249">
+        <f>POWER(2,ItemStatCost!V249)-ItemStatCost!W249</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>432</v>
+      </c>
+      <c r="B250">
+        <f>-ItemStatCost!W250</f>
+        <v>0</v>
+      </c>
+      <c r="C250">
+        <f>POWER(2,ItemStatCost!V250)-ItemStatCost!W250</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
+        <v>433</v>
+      </c>
+      <c r="B251">
+        <f>-ItemStatCost!W251</f>
+        <v>0</v>
+      </c>
+      <c r="C251">
+        <f>POWER(2,ItemStatCost!V251)-ItemStatCost!W251</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
+        <v>434</v>
+      </c>
+      <c r="B252">
+        <f>-ItemStatCost!W252</f>
+        <v>0</v>
+      </c>
+      <c r="C252">
+        <f>POWER(2,ItemStatCost!V252)-ItemStatCost!W252</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
+        <v>435</v>
+      </c>
+      <c r="B253">
+        <f>-ItemStatCost!W253</f>
+        <v>0</v>
+      </c>
+      <c r="C253">
+        <f>POWER(2,ItemStatCost!V253)-ItemStatCost!W253</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
+        <v>436</v>
+      </c>
+      <c r="B254">
+        <f>-ItemStatCost!W254</f>
+        <v>0</v>
+      </c>
+      <c r="C254">
+        <f>POWER(2,ItemStatCost!V254)-ItemStatCost!W254</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
+        <v>438</v>
+      </c>
+      <c r="B255">
+        <f>-ItemStatCost!W255</f>
+        <v>0</v>
+      </c>
+      <c r="C255">
+        <f>POWER(2,ItemStatCost!V255)-ItemStatCost!W255</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
+        <v>440</v>
+      </c>
+      <c r="B256">
+        <f>-ItemStatCost!W256</f>
+        <v>0</v>
+      </c>
+      <c r="C256">
+        <f>POWER(2,ItemStatCost!V256)-ItemStatCost!W256</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A257" t="s">
+        <v>442</v>
+      </c>
+      <c r="B257">
+        <f>-ItemStatCost!W257</f>
+        <v>0</v>
+      </c>
+      <c r="C257">
+        <f>POWER(2,ItemStatCost!V257)-ItemStatCost!W257</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A258" t="s">
+        <v>443</v>
+      </c>
+      <c r="B258">
+        <f>-ItemStatCost!W258</f>
+        <v>0</v>
+      </c>
+      <c r="C258">
+        <f>POWER(2,ItemStatCost!V258)-ItemStatCost!W258</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A259" t="s">
+        <v>444</v>
+      </c>
+      <c r="B259">
+        <f>-ItemStatCost!W259</f>
+        <v>0</v>
+      </c>
+      <c r="C259">
+        <f>POWER(2,ItemStatCost!V259)-ItemStatCost!W259</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A260" t="s">
+        <v>445</v>
+      </c>
+      <c r="B260">
+        <f>-ItemStatCost!W260</f>
+        <v>0</v>
+      </c>
+      <c r="C260">
+        <f>POWER(2,ItemStatCost!V260)-ItemStatCost!W260</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A261" t="s">
+        <v>446</v>
+      </c>
+      <c r="B261">
+        <f>-ItemStatCost!W261</f>
+        <v>0</v>
+      </c>
+      <c r="C261">
+        <f>POWER(2,ItemStatCost!V261)-ItemStatCost!W261</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A262" t="s">
+        <v>447</v>
+      </c>
+      <c r="B262">
+        <f>-ItemStatCost!W262</f>
+        <v>0</v>
+      </c>
+      <c r="C262">
+        <f>POWER(2,ItemStatCost!V262)-ItemStatCost!W262</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A263" t="s">
+        <v>448</v>
+      </c>
+      <c r="B263">
+        <f>-ItemStatCost!W263</f>
+        <v>0</v>
+      </c>
+      <c r="C263">
+        <f>POWER(2,ItemStatCost!V263)-ItemStatCost!W263</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A264" t="s">
+        <v>449</v>
+      </c>
+      <c r="B264">
+        <f>-ItemStatCost!W264</f>
+        <v>0</v>
+      </c>
+      <c r="C264">
+        <f>POWER(2,ItemStatCost!V264)-ItemStatCost!W264</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A265" t="s">
+        <v>450</v>
+      </c>
+      <c r="B265">
+        <f>-ItemStatCost!W265</f>
+        <v>0</v>
+      </c>
+      <c r="C265">
+        <f>POWER(2,ItemStatCost!V265)-ItemStatCost!W265</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A266" t="s">
+        <v>451</v>
+      </c>
+      <c r="B266">
+        <f>-ItemStatCost!W266</f>
+        <v>0</v>
+      </c>
+      <c r="C266">
+        <f>POWER(2,ItemStatCost!V266)-ItemStatCost!W266</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A267" t="s">
+        <v>452</v>
+      </c>
+      <c r="B267">
+        <f>-ItemStatCost!W267</f>
+        <v>0</v>
+      </c>
+      <c r="C267">
+        <f>POWER(2,ItemStatCost!V267)-ItemStatCost!W267</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A268" t="s">
+        <v>453</v>
+      </c>
+      <c r="B268">
+        <f>-ItemStatCost!W268</f>
+        <v>0</v>
+      </c>
+      <c r="C268">
+        <f>POWER(2,ItemStatCost!V268)-ItemStatCost!W268</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A269" t="s">
+        <v>454</v>
+      </c>
+      <c r="B269">
+        <f>-ItemStatCost!W269</f>
+        <v>0</v>
+      </c>
+      <c r="C269">
+        <f>POWER(2,ItemStatCost!V269)-ItemStatCost!W269</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A270" t="s">
+        <v>455</v>
+      </c>
+      <c r="B270">
+        <f>-ItemStatCost!W270</f>
+        <v>0</v>
+      </c>
+      <c r="C270">
+        <f>POWER(2,ItemStatCost!V270)-ItemStatCost!W270</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A271" t="s">
+        <v>456</v>
+      </c>
+      <c r="B271">
+        <f>-ItemStatCost!W271</f>
+        <v>0</v>
+      </c>
+      <c r="C271">
+        <f>POWER(2,ItemStatCost!V271)-ItemStatCost!W271</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A272" t="s">
+        <v>457</v>
+      </c>
+      <c r="B272">
+        <f>-ItemStatCost!W272</f>
+        <v>0</v>
+      </c>
+      <c r="C272">
+        <f>POWER(2,ItemStatCost!V272)-ItemStatCost!W272</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A273" t="s">
+        <v>458</v>
+      </c>
+      <c r="B273">
+        <f>-ItemStatCost!W273</f>
+        <v>0</v>
+      </c>
+      <c r="C273">
+        <f>POWER(2,ItemStatCost!V273)-ItemStatCost!W273</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A274" t="s">
+        <v>459</v>
+      </c>
+      <c r="B274">
+        <f>-ItemStatCost!W274</f>
+        <v>0</v>
+      </c>
+      <c r="C274">
+        <f>POWER(2,ItemStatCost!V274)-ItemStatCost!W274</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A275" t="s">
+        <v>460</v>
+      </c>
+      <c r="B275">
+        <f>-ItemStatCost!W275</f>
+        <v>0</v>
+      </c>
+      <c r="C275">
+        <f>POWER(2,ItemStatCost!V275)-ItemStatCost!W275</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A276" t="s">
+        <v>461</v>
+      </c>
+      <c r="B276">
+        <f>-ItemStatCost!W276</f>
+        <v>0</v>
+      </c>
+      <c r="C276">
+        <f>POWER(2,ItemStatCost!V276)-ItemStatCost!W276</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A277" t="s">
+        <v>462</v>
+      </c>
+      <c r="B277">
+        <f>-ItemStatCost!W277</f>
+        <v>0</v>
+      </c>
+      <c r="C277">
+        <f>POWER(2,ItemStatCost!V277)-ItemStatCost!W277</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A278" t="s">
+        <v>463</v>
+      </c>
+      <c r="B278">
+        <f>-ItemStatCost!W278</f>
+        <v>0</v>
+      </c>
+      <c r="C278">
+        <f>POWER(2,ItemStatCost!V278)-ItemStatCost!W278</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A279" t="s">
+        <v>464</v>
+      </c>
+      <c r="B279">
+        <f>-ItemStatCost!W279</f>
+        <v>0</v>
+      </c>
+      <c r="C279">
+        <f>POWER(2,ItemStatCost!V279)-ItemStatCost!W279</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A280" t="s">
+        <v>465</v>
+      </c>
+      <c r="B280">
+        <f>-ItemStatCost!W280</f>
+        <v>0</v>
+      </c>
+      <c r="C280">
+        <f>POWER(2,ItemStatCost!V280)-ItemStatCost!W280</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A281" t="s">
+        <v>466</v>
+      </c>
+      <c r="B281">
+        <f>-ItemStatCost!W281</f>
+        <v>0</v>
+      </c>
+      <c r="C281">
+        <f>POWER(2,ItemStatCost!V281)-ItemStatCost!W281</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A282" t="s">
+        <v>467</v>
+      </c>
+      <c r="B282">
+        <f>-ItemStatCost!W282</f>
+        <v>0</v>
+      </c>
+      <c r="C282">
+        <f>POWER(2,ItemStatCost!V282)-ItemStatCost!W282</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A283" t="s">
+        <v>468</v>
+      </c>
+      <c r="B283">
+        <f>-ItemStatCost!W283</f>
+        <v>0</v>
+      </c>
+      <c r="C283">
+        <f>POWER(2,ItemStatCost!V283)-ItemStatCost!W283</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A284" t="s">
+        <v>469</v>
+      </c>
+      <c r="B284">
+        <f>-ItemStatCost!W284</f>
+        <v>0</v>
+      </c>
+      <c r="C284">
+        <f>POWER(2,ItemStatCost!V284)-ItemStatCost!W284</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A285" t="s">
+        <v>470</v>
+      </c>
+      <c r="B285">
+        <f>-ItemStatCost!W285</f>
+        <v>0</v>
+      </c>
+      <c r="C285">
+        <f>POWER(2,ItemStatCost!V285)-ItemStatCost!W285</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A286" t="s">
+        <v>471</v>
+      </c>
+      <c r="B286">
+        <f>-ItemStatCost!W286</f>
+        <v>0</v>
+      </c>
+      <c r="C286">
+        <f>POWER(2,ItemStatCost!V286)-ItemStatCost!W286</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A287" t="s">
+        <v>472</v>
+      </c>
+      <c r="B287">
+        <f>-ItemStatCost!W287</f>
+        <v>0</v>
+      </c>
+      <c r="C287">
+        <f>POWER(2,ItemStatCost!V287)-ItemStatCost!W287</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A288" t="s">
+        <v>473</v>
+      </c>
+      <c r="B288">
+        <f>-ItemStatCost!W288</f>
+        <v>0</v>
+      </c>
+      <c r="C288">
+        <f>POWER(2,ItemStatCost!V288)-ItemStatCost!W288</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A289" t="s">
+        <v>474</v>
+      </c>
+      <c r="B289">
+        <f>-ItemStatCost!W289</f>
+        <v>0</v>
+      </c>
+      <c r="C289">
+        <f>POWER(2,ItemStatCost!V289)-ItemStatCost!W289</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A290" t="s">
+        <v>475</v>
+      </c>
+      <c r="B290">
+        <f>-ItemStatCost!W290</f>
+        <v>0</v>
+      </c>
+      <c r="C290">
+        <f>POWER(2,ItemStatCost!V290)-ItemStatCost!W290</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A291" t="s">
+        <v>476</v>
+      </c>
+      <c r="B291">
+        <f>-ItemStatCost!W291</f>
+        <v>0</v>
+      </c>
+      <c r="C291">
+        <f>POWER(2,ItemStatCost!V291)-ItemStatCost!W291</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A292" t="s">
+        <v>477</v>
+      </c>
+      <c r="B292">
+        <f>-ItemStatCost!W292</f>
+        <v>0</v>
+      </c>
+      <c r="C292">
+        <f>POWER(2,ItemStatCost!V292)-ItemStatCost!W292</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A293" t="s">
+        <v>478</v>
+      </c>
+      <c r="B293">
+        <f>-ItemStatCost!W293</f>
+        <v>0</v>
+      </c>
+      <c r="C293">
+        <f>POWER(2,ItemStatCost!V293)-ItemStatCost!W293</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A294" t="s">
+        <v>479</v>
+      </c>
+      <c r="B294">
+        <f>-ItemStatCost!W294</f>
+        <v>0</v>
+      </c>
+      <c r="C294">
+        <f>POWER(2,ItemStatCost!V294)-ItemStatCost!W294</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A295" t="s">
+        <v>480</v>
+      </c>
+      <c r="B295">
+        <f>-ItemStatCost!W295</f>
+        <v>0</v>
+      </c>
+      <c r="C295">
+        <f>POWER(2,ItemStatCost!V295)-ItemStatCost!W295</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A296" t="s">
+        <v>481</v>
+      </c>
+      <c r="B296">
+        <f>-ItemStatCost!W296</f>
+        <v>0</v>
+      </c>
+      <c r="C296">
+        <f>POWER(2,ItemStatCost!V296)-ItemStatCost!W296</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A297" t="s">
+        <v>482</v>
+      </c>
+      <c r="B297">
+        <f>-ItemStatCost!W297</f>
+        <v>0</v>
+      </c>
+      <c r="C297">
+        <f>POWER(2,ItemStatCost!V297)-ItemStatCost!W297</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A298" t="s">
+        <v>483</v>
+      </c>
+      <c r="B298">
+        <f>-ItemStatCost!W298</f>
+        <v>0</v>
+      </c>
+      <c r="C298">
+        <f>POWER(2,ItemStatCost!V298)-ItemStatCost!W298</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A299" t="s">
+        <v>484</v>
+      </c>
+      <c r="B299">
+        <f>-ItemStatCost!W299</f>
+        <v>0</v>
+      </c>
+      <c r="C299">
+        <f>POWER(2,ItemStatCost!V299)-ItemStatCost!W299</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A300" t="s">
+        <v>485</v>
+      </c>
+      <c r="B300">
+        <f>-ItemStatCost!W300</f>
+        <v>0</v>
+      </c>
+      <c r="C300">
+        <f>POWER(2,ItemStatCost!V300)-ItemStatCost!W300</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A301" t="s">
+        <v>486</v>
+      </c>
+      <c r="B301">
+        <f>-ItemStatCost!W301</f>
+        <v>0</v>
+      </c>
+      <c r="C301">
+        <f>POWER(2,ItemStatCost!V301)-ItemStatCost!W301</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A302" t="s">
+        <v>487</v>
+      </c>
+      <c r="B302">
+        <f>-ItemStatCost!W302</f>
+        <v>0</v>
+      </c>
+      <c r="C302">
+        <f>POWER(2,ItemStatCost!V302)-ItemStatCost!W302</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A303" t="s">
+        <v>488</v>
+      </c>
+      <c r="B303">
+        <f>-ItemStatCost!W303</f>
+        <v>0</v>
+      </c>
+      <c r="C303">
+        <f>POWER(2,ItemStatCost!V303)-ItemStatCost!W303</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A304" t="s">
+        <v>489</v>
+      </c>
+      <c r="B304">
+        <f>-ItemStatCost!W304</f>
+        <v>0</v>
+      </c>
+      <c r="C304">
+        <f>POWER(2,ItemStatCost!V304)-ItemStatCost!W304</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A305" t="s">
+        <v>490</v>
+      </c>
+      <c r="B305">
+        <f>-ItemStatCost!W305</f>
+        <v>0</v>
+      </c>
+      <c r="C305">
+        <f>POWER(2,ItemStatCost!V305)-ItemStatCost!W305</f>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A306" t="s">
+        <v>491</v>
+      </c>
+      <c r="B306">
+        <f>-ItemStatCost!W306</f>
+        <v>0</v>
+      </c>
+      <c r="C306">
+        <f>POWER(2,ItemStatCost!V306)-ItemStatCost!W306</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A307" t="s">
+        <v>492</v>
+      </c>
+      <c r="B307">
+        <f>-ItemStatCost!W307</f>
+        <v>-50</v>
+      </c>
+      <c r="C307">
+        <f>POWER(2,ItemStatCost!V307)-ItemStatCost!W307</f>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A308" t="s">
+        <v>494</v>
+      </c>
+      <c r="B308">
+        <f>-ItemStatCost!W308</f>
+        <v>-50</v>
+      </c>
+      <c r="C308">
+        <f>POWER(2,ItemStatCost!V308)-ItemStatCost!W308</f>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A309" t="s">
+        <v>496</v>
+      </c>
+      <c r="B309">
+        <f>-ItemStatCost!W309</f>
+        <v>-50</v>
+      </c>
+      <c r="C309">
+        <f>POWER(2,ItemStatCost!V309)-ItemStatCost!W309</f>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A310" t="s">
+        <v>498</v>
+      </c>
+      <c r="B310">
+        <f>-ItemStatCost!W310</f>
+        <v>-50</v>
+      </c>
+      <c r="C310">
+        <f>POWER(2,ItemStatCost!V310)-ItemStatCost!W310</f>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A311" t="s">
+        <v>500</v>
+      </c>
+      <c r="B311">
+        <f>-ItemStatCost!W311</f>
+        <v>0</v>
+      </c>
+      <c r="C311">
+        <f>POWER(2,ItemStatCost!V311)-ItemStatCost!W311</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A312" t="s">
+        <v>501</v>
+      </c>
+      <c r="B312">
+        <f>-ItemStatCost!W312</f>
+        <v>0</v>
+      </c>
+      <c r="C312">
+        <f>POWER(2,ItemStatCost!V312)-ItemStatCost!W312</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A313" t="s">
+        <v>502</v>
+      </c>
+      <c r="B313">
+        <f>-ItemStatCost!W313</f>
+        <v>0</v>
+      </c>
+      <c r="C313">
+        <f>POWER(2,ItemStatCost!V313)-ItemStatCost!W313</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A314" t="s">
+        <v>503</v>
+      </c>
+      <c r="B314">
+        <f>-ItemStatCost!W314</f>
+        <v>0</v>
+      </c>
+      <c r="C314">
+        <f>POWER(2,ItemStatCost!V314)-ItemStatCost!W314</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A315" t="s">
+        <v>504</v>
+      </c>
+      <c r="B315">
+        <f>-ItemStatCost!W315</f>
+        <v>0</v>
+      </c>
+      <c r="C315">
+        <f>POWER(2,ItemStatCost!V315)-ItemStatCost!W315</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A316" t="s">
+        <v>505</v>
+      </c>
+      <c r="B316">
+        <f>-ItemStatCost!W316</f>
+        <v>0</v>
+      </c>
+      <c r="C316">
+        <f>POWER(2,ItemStatCost!V316)-ItemStatCost!W316</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A317" t="s">
+        <v>506</v>
+      </c>
+      <c r="B317">
+        <f>-ItemStatCost!W317</f>
+        <v>0</v>
+      </c>
+      <c r="C317">
+        <f>POWER(2,ItemStatCost!V317)-ItemStatCost!W317</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A318" t="s">
+        <v>507</v>
+      </c>
+      <c r="B318">
+        <f>-ItemStatCost!W318</f>
+        <v>0</v>
+      </c>
+      <c r="C318">
+        <f>POWER(2,ItemStatCost!V318)-ItemStatCost!W318</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A319" t="s">
+        <v>508</v>
+      </c>
+      <c r="B319">
+        <f>-ItemStatCost!W319</f>
+        <v>0</v>
+      </c>
+      <c r="C319">
+        <f>POWER(2,ItemStatCost!V319)-ItemStatCost!W319</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A320" t="s">
+        <v>509</v>
+      </c>
+      <c r="B320">
+        <f>-ItemStatCost!W320</f>
+        <v>0</v>
+      </c>
+      <c r="C320">
+        <f>POWER(2,ItemStatCost!V320)-ItemStatCost!W320</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A321" t="s">
+        <v>510</v>
+      </c>
+      <c r="B321">
+        <f>-ItemStatCost!W321</f>
+        <v>0</v>
+      </c>
+      <c r="C321">
+        <f>POWER(2,ItemStatCost!V321)-ItemStatCost!W321</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A322" t="s">
+        <v>511</v>
+      </c>
+      <c r="B322">
+        <f>-ItemStatCost!W322</f>
+        <v>0</v>
+      </c>
+      <c r="C322">
+        <f>POWER(2,ItemStatCost!V322)-ItemStatCost!W322</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A323" t="s">
+        <v>512</v>
+      </c>
+      <c r="B323">
+        <f>-ItemStatCost!W323</f>
+        <v>0</v>
+      </c>
+      <c r="C323">
+        <f>POWER(2,ItemStatCost!V323)-ItemStatCost!W323</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A324" t="s">
+        <v>513</v>
+      </c>
+      <c r="B324">
+        <f>-ItemStatCost!W324</f>
+        <v>0</v>
+      </c>
+      <c r="C324">
+        <f>POWER(2,ItemStatCost!V324)-ItemStatCost!W324</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A325" t="s">
+        <v>514</v>
+      </c>
+      <c r="B325">
+        <f>-ItemStatCost!W325</f>
+        <v>0</v>
+      </c>
+      <c r="C325">
+        <f>POWER(2,ItemStatCost!V325)-ItemStatCost!W325</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A326" t="s">
+        <v>515</v>
+      </c>
+      <c r="B326">
+        <f>-ItemStatCost!W326</f>
+        <v>0</v>
+      </c>
+      <c r="C326">
+        <f>POWER(2,ItemStatCost!V326)-ItemStatCost!W326</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A327" t="s">
+        <v>516</v>
+      </c>
+      <c r="B327">
+        <f>-ItemStatCost!W327</f>
+        <v>0</v>
+      </c>
+      <c r="C327">
+        <f>POWER(2,ItemStatCost!V327)-ItemStatCost!W327</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A328" t="s">
+        <v>517</v>
+      </c>
+      <c r="B328">
+        <f>-ItemStatCost!W328</f>
+        <v>0</v>
+      </c>
+      <c r="C328">
+        <f>POWER(2,ItemStatCost!V328)-ItemStatCost!W328</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A329" t="s">
+        <v>518</v>
+      </c>
+      <c r="B329">
+        <f>-ItemStatCost!W329</f>
+        <v>0</v>
+      </c>
+      <c r="C329">
+        <f>POWER(2,ItemStatCost!V329)-ItemStatCost!W329</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A330" t="s">
+        <v>519</v>
+      </c>
+      <c r="B330">
+        <f>-ItemStatCost!W330</f>
+        <v>0</v>
+      </c>
+      <c r="C330">
+        <f>POWER(2,ItemStatCost!V330)-ItemStatCost!W330</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A331" t="s">
+        <v>520</v>
+      </c>
+      <c r="B331">
+        <f>-ItemStatCost!W331</f>
+        <v>-50</v>
+      </c>
+      <c r="C331">
+        <f>POWER(2,ItemStatCost!V331)-ItemStatCost!W331</f>
+        <v>462</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A332" t="s">
+        <v>522</v>
+      </c>
+      <c r="B332">
+        <f>-ItemStatCost!W332</f>
+        <v>-50</v>
+      </c>
+      <c r="C332">
+        <f>POWER(2,ItemStatCost!V332)-ItemStatCost!W332</f>
+        <v>462</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A333" t="s">
+        <v>524</v>
+      </c>
+      <c r="B333">
+        <f>-ItemStatCost!W333</f>
+        <v>-50</v>
+      </c>
+      <c r="C333">
+        <f>POWER(2,ItemStatCost!V333)-ItemStatCost!W333</f>
+        <v>462</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A334" t="s">
+        <v>526</v>
+      </c>
+      <c r="B334">
+        <f>-ItemStatCost!W334</f>
+        <v>-50</v>
+      </c>
+      <c r="C334">
+        <f>POWER(2,ItemStatCost!V334)-ItemStatCost!W334</f>
+        <v>462</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A335" t="s">
+        <v>528</v>
+      </c>
+      <c r="B335">
+        <f>-ItemStatCost!W335</f>
+        <v>0</v>
+      </c>
+      <c r="C335">
+        <f>POWER(2,ItemStatCost!V335)-ItemStatCost!W335</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A336" t="s">
+        <v>529</v>
+      </c>
+      <c r="B336">
+        <f>-ItemStatCost!W336</f>
+        <v>0</v>
+      </c>
+      <c r="C336">
+        <f>POWER(2,ItemStatCost!V336)-ItemStatCost!W336</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A337" t="s">
+        <v>530</v>
+      </c>
+      <c r="B337">
+        <f>-ItemStatCost!W337</f>
+        <v>0</v>
+      </c>
+      <c r="C337">
+        <f>POWER(2,ItemStatCost!V337)-ItemStatCost!W337</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A338" t="s">
+        <v>531</v>
+      </c>
+      <c r="B338">
+        <f>-ItemStatCost!W338</f>
+        <v>0</v>
+      </c>
+      <c r="C338">
+        <f>POWER(2,ItemStatCost!V338)-ItemStatCost!W338</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A339" t="s">
+        <v>532</v>
+      </c>
+      <c r="B339">
+        <f>-ItemStatCost!W339</f>
+        <v>0</v>
+      </c>
+      <c r="C339">
+        <f>POWER(2,ItemStatCost!V339)-ItemStatCost!W339</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A340" t="s">
+        <v>533</v>
+      </c>
+      <c r="B340">
+        <f>-ItemStatCost!W340</f>
+        <v>0</v>
+      </c>
+      <c r="C340">
+        <f>POWER(2,ItemStatCost!V340)-ItemStatCost!W340</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A341" t="s">
+        <v>534</v>
+      </c>
+      <c r="B341">
+        <f>-ItemStatCost!W341</f>
+        <v>0</v>
+      </c>
+      <c r="C341">
+        <f>POWER(2,ItemStatCost!V341)-ItemStatCost!W341</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A342" t="s">
+        <v>535</v>
+      </c>
+      <c r="B342">
+        <f>-ItemStatCost!W342</f>
+        <v>0</v>
+      </c>
+      <c r="C342">
+        <f>POWER(2,ItemStatCost!V342)-ItemStatCost!W342</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A343" t="s">
+        <v>536</v>
+      </c>
+      <c r="B343">
+        <f>-ItemStatCost!W343</f>
+        <v>0</v>
+      </c>
+      <c r="C343">
+        <f>POWER(2,ItemStatCost!V343)-ItemStatCost!W343</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A344" t="s">
+        <v>537</v>
+      </c>
+      <c r="B344">
+        <f>-ItemStatCost!W344</f>
+        <v>0</v>
+      </c>
+      <c r="C344">
+        <f>POWER(2,ItemStatCost!V344)-ItemStatCost!W344</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A345" t="s">
+        <v>538</v>
+      </c>
+      <c r="B345">
+        <f>-ItemStatCost!W345</f>
+        <v>0</v>
+      </c>
+      <c r="C345">
+        <f>POWER(2,ItemStatCost!V345)-ItemStatCost!W345</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A346" t="s">
+        <v>539</v>
+      </c>
+      <c r="B346">
+        <f>-ItemStatCost!W346</f>
+        <v>0</v>
+      </c>
+      <c r="C346">
+        <f>POWER(2,ItemStatCost!V346)-ItemStatCost!W346</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A347" t="s">
+        <v>540</v>
+      </c>
+      <c r="B347">
+        <f>-ItemStatCost!W347</f>
+        <v>0</v>
+      </c>
+      <c r="C347">
+        <f>POWER(2,ItemStatCost!V347)-ItemStatCost!W347</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A348" t="s">
+        <v>541</v>
+      </c>
+      <c r="B348">
+        <f>-ItemStatCost!W348</f>
+        <v>0</v>
+      </c>
+      <c r="C348">
+        <f>POWER(2,ItemStatCost!V348)-ItemStatCost!W348</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="349" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A349" t="s">
+        <v>542</v>
+      </c>
+      <c r="B349">
+        <f>-ItemStatCost!W349</f>
+        <v>0</v>
+      </c>
+      <c r="C349">
+        <f>POWER(2,ItemStatCost!V349)-ItemStatCost!W349</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A350" t="s">
+        <v>543</v>
+      </c>
+      <c r="B350">
+        <f>-ItemStatCost!W350</f>
+        <v>0</v>
+      </c>
+      <c r="C350">
+        <f>POWER(2,ItemStatCost!V350)-ItemStatCost!W350</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A351" t="s">
+        <v>544</v>
+      </c>
+      <c r="B351">
+        <f>-ItemStatCost!W351</f>
+        <v>0</v>
+      </c>
+      <c r="C351">
+        <f>POWER(2,ItemStatCost!V351)-ItemStatCost!W351</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="352" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A352" t="s">
+        <v>545</v>
+      </c>
+      <c r="B352">
+        <f>-ItemStatCost!W352</f>
+        <v>0</v>
+      </c>
+      <c r="C352">
+        <f>POWER(2,ItemStatCost!V352)-ItemStatCost!W352</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A353" t="s">
+        <v>546</v>
+      </c>
+      <c r="B353">
+        <f>-ItemStatCost!W353</f>
+        <v>0</v>
+      </c>
+      <c r="C353">
+        <f>POWER(2,ItemStatCost!V353)-ItemStatCost!W353</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A354" t="s">
+        <v>547</v>
+      </c>
+      <c r="B354">
+        <f>-ItemStatCost!W354</f>
+        <v>0</v>
+      </c>
+      <c r="C354">
+        <f>POWER(2,ItemStatCost!V354)-ItemStatCost!W354</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A355" t="s">
+        <v>548</v>
+      </c>
+      <c r="B355">
+        <f>-ItemStatCost!W355</f>
+        <v>0</v>
+      </c>
+      <c r="C355">
+        <f>POWER(2,ItemStatCost!V355)-ItemStatCost!W355</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A356" t="s">
+        <v>549</v>
+      </c>
+      <c r="B356">
+        <f>-ItemStatCost!W356</f>
+        <v>0</v>
+      </c>
+      <c r="C356">
+        <f>POWER(2,ItemStatCost!V356)-ItemStatCost!W356</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A357" t="s">
+        <v>550</v>
+      </c>
+      <c r="B357">
+        <f>-ItemStatCost!W357</f>
+        <v>0</v>
+      </c>
+      <c r="C357">
+        <f>POWER(2,ItemStatCost!V357)-ItemStatCost!W357</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A358" t="s">
+        <v>551</v>
+      </c>
+      <c r="B358">
+        <f>-ItemStatCost!W358</f>
+        <v>0</v>
+      </c>
+      <c r="C358">
+        <f>POWER(2,ItemStatCost!V358)-ItemStatCost!W358</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A359" t="s">
+        <v>552</v>
+      </c>
+      <c r="B359">
+        <f>-ItemStatCost!W359</f>
+        <v>-50</v>
+      </c>
+      <c r="C359">
+        <f>POWER(2,ItemStatCost!V359)-ItemStatCost!W359</f>
+        <v>462</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A360" t="s">
+        <v>553</v>
+      </c>
+      <c r="B360">
+        <f>-ItemStatCost!W360</f>
+        <v>0</v>
+      </c>
+      <c r="C360">
+        <f>POWER(2,ItemStatCost!V360)-ItemStatCost!W360</f>
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>